<commit_message>
add more site domains
</commit_message>
<xml_diff>
--- a/domains.xlsx
+++ b/domains.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -36,16 +36,94 @@
     <t>Time added</t>
   </si>
   <si>
-    <t>202522-1625</t>
-  </si>
-  <si>
-    <t>Media-News</t>
+    <t>2025-1</t>
+  </si>
+  <si>
+    <t>News-Media</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>https://rebaltica.lv/</t>
+  </si>
+  <si>
+    <t>2025-2</t>
+  </si>
+  <si>
+    <t>NEWS</t>
+  </si>
+  <si>
+    <t>https://testpress.news/</t>
+  </si>
+  <si>
+    <t>2025-3</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>https://kasta.ua/</t>
+  </si>
+  <si>
+    <t>2025-4</t>
+  </si>
+  <si>
+    <t>Foto</t>
+  </si>
+  <si>
+    <t>https://www.unfoto.lv/</t>
+  </si>
+  <si>
+    <t>2025-5</t>
+  </si>
+  <si>
+    <t>Edu</t>
+  </si>
+  <si>
+    <t>EDU</t>
+  </si>
+  <si>
+    <t>https://www.harvard.edu/</t>
+  </si>
+  <si>
+    <t>2025-6</t>
+  </si>
+  <si>
+    <t>Gov</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>https://www.gov.pl/web/diplomacy</t>
+  </si>
+  <si>
+    <t>2025-7</t>
+  </si>
+  <si>
+    <t>Adult</t>
   </si>
   <si>
     <t>COM</t>
   </si>
   <si>
-    <t>https://www.harvard.edu/</t>
+    <t>https://fapello.com/</t>
+  </si>
+  <si>
+    <t>2025-8</t>
+  </si>
+  <si>
+    <t>https://www.aljazeera.com/</t>
+  </si>
+  <si>
+    <t>2025-9</t>
+  </si>
+  <si>
+    <t>https://www.bbc.com/</t>
   </si>
 </sst>
 </file>
@@ -63,7 +141,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -95,9 +173,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -107,7 +188,7 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,14 +498,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="38.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="38.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -454,107 +535,187 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
-        <v>45710</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="E2" s="3">
+        <v>45703</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3">
+        <v>45703</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45703</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3">
+        <v>45703</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3">
+        <v>45703</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3">
+        <v>45703</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3">
+        <v>45703</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3">
+        <v>45705</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="3">
+        <v>45705</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="E11" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="E12" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="E13" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="E14" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="E15" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>